<commit_message>
Game iterations testing e.g
</commit_message>
<xml_diff>
--- a/src/test_results.xlsx
+++ b/src/test_results.xlsx
@@ -8,15 +8,18 @@
   </bookViews>
   <sheets>
     <sheet name="test1" sheetId="1" r:id="rId1"/>
-    <sheet name="Ark2" sheetId="2" r:id="rId2"/>
+    <sheet name="compare1" sheetId="2" r:id="rId2"/>
     <sheet name="Ark3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">test1!$A$5:$E$5</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>Time begin</t>
   </si>
@@ -32,12 +35,21 @@
   <si>
     <t>Time taken to play out game</t>
   </si>
+  <si>
+    <t>Latrunculi</t>
+  </si>
+  <si>
+    <t>Latrunculi_ne</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,16 +65,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -70,15 +94,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -371,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A5:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD15"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15"/>
@@ -383,24 +435,25 @@
     <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="5" spans="1:5" s="1" customFormat="1">
+      <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A5:E5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -408,14 +461,385 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A4:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="str">
+        <f>IF(test1!$C6=$A$4,test1!$D6,"")</f>
+        <v/>
+      </c>
+      <c r="B6" t="str">
+        <f>IF(test1!$C6=$A$4,test1!$E6,"")</f>
+        <v/>
+      </c>
+      <c r="D6" t="str">
+        <f>IF(test1!$C6=$D$4,test1!$D6,"")</f>
+        <v/>
+      </c>
+      <c r="E6" t="str">
+        <f>IF(test1!$C6=$D$4,test1!$E6,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="str">
+        <f>IF(test1!$C7=$A$4,test1!$D7,"")</f>
+        <v/>
+      </c>
+      <c r="B7" t="str">
+        <f>IF(test1!$C7=$A$4,test1!$E7,"")</f>
+        <v/>
+      </c>
+      <c r="D7" t="str">
+        <f>IF(test1!$C7=$D$4,test1!$D7,"")</f>
+        <v/>
+      </c>
+      <c r="E7" t="str">
+        <f>IF(test1!$C7=$D$4,test1!$E7,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="str">
+        <f>IF(test1!$C8=$A$4,test1!$D8,"")</f>
+        <v/>
+      </c>
+      <c r="B8" t="str">
+        <f>IF(test1!$C8=$A$4,test1!$E8,"")</f>
+        <v/>
+      </c>
+      <c r="D8" t="str">
+        <f>IF(test1!$C8=$D$4,test1!$D8,"")</f>
+        <v/>
+      </c>
+      <c r="E8" t="str">
+        <f>IF(test1!$C8=$D$4,test1!$E8,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="str">
+        <f>IF(test1!$C9=$A$4,test1!$D9,"")</f>
+        <v/>
+      </c>
+      <c r="B9" t="str">
+        <f>IF(test1!$C9=$A$4,test1!$E9,"")</f>
+        <v/>
+      </c>
+      <c r="D9" t="str">
+        <f>IF(test1!$C9=$D$4,test1!$D9,"")</f>
+        <v/>
+      </c>
+      <c r="E9" t="str">
+        <f>IF(test1!$C9=$D$4,test1!$E9,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="str">
+        <f>IF(test1!$C10=$A$4,test1!$D10,"")</f>
+        <v/>
+      </c>
+      <c r="B10" t="str">
+        <f>IF(test1!$C10=$A$4,test1!$E10,"")</f>
+        <v/>
+      </c>
+      <c r="D10" t="str">
+        <f>IF(test1!$C10=$D$4,test1!$D10,"")</f>
+        <v/>
+      </c>
+      <c r="E10" t="str">
+        <f>IF(test1!$C10=$D$4,test1!$E10,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="str">
+        <f>IF(test1!$C11=$A$4,test1!$D11,"")</f>
+        <v/>
+      </c>
+      <c r="B11" t="str">
+        <f>IF(test1!$C11=$A$4,test1!$E11,"")</f>
+        <v/>
+      </c>
+      <c r="D11" t="str">
+        <f>IF(test1!$C11=$D$4,test1!$D11,"")</f>
+        <v/>
+      </c>
+      <c r="E11" t="str">
+        <f>IF(test1!$C11=$D$4,test1!$E11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="str">
+        <f>IF(test1!$C12=$A$4,test1!$D12,"")</f>
+        <v/>
+      </c>
+      <c r="B12" t="str">
+        <f>IF(test1!$C12=$A$4,test1!$E12,"")</f>
+        <v/>
+      </c>
+      <c r="D12" t="str">
+        <f>IF(test1!$C12=$D$4,test1!$D12,"")</f>
+        <v/>
+      </c>
+      <c r="E12" t="str">
+        <f>IF(test1!$C12=$D$4,test1!$E12,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="str">
+        <f>IF(test1!$C13=$A$4,test1!$D13,"")</f>
+        <v/>
+      </c>
+      <c r="B13" t="str">
+        <f>IF(test1!$C13=$A$4,test1!$E13,"")</f>
+        <v/>
+      </c>
+      <c r="D13" t="str">
+        <f>IF(test1!$C13=$D$4,test1!$D13,"")</f>
+        <v/>
+      </c>
+      <c r="E13" t="str">
+        <f>IF(test1!$C13=$D$4,test1!$E13,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="str">
+        <f>IF(test1!$C14=$A$4,test1!$D14,"")</f>
+        <v/>
+      </c>
+      <c r="B14" t="str">
+        <f>IF(test1!$C14=$A$4,test1!$E14,"")</f>
+        <v/>
+      </c>
+      <c r="D14" t="str">
+        <f>IF(test1!$C14=$D$4,test1!$D14,"")</f>
+        <v/>
+      </c>
+      <c r="E14" t="str">
+        <f>IF(test1!$C14=$D$4,test1!$E14,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="str">
+        <f>IF(test1!$C15=$A$4,test1!$D15,"")</f>
+        <v/>
+      </c>
+      <c r="B15" t="str">
+        <f>IF(test1!$C15=$A$4,test1!$E15,"")</f>
+        <v/>
+      </c>
+      <c r="D15" t="str">
+        <f>IF(test1!$C15=$D$4,test1!$D15,"")</f>
+        <v/>
+      </c>
+      <c r="E15" t="str">
+        <f>IF(test1!$C15=$D$4,test1!$E15,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="str">
+        <f>IF(test1!$C16=$A$4,test1!$D16,"")</f>
+        <v/>
+      </c>
+      <c r="B16" t="str">
+        <f>IF(test1!$C16=$A$4,test1!$E16,"")</f>
+        <v/>
+      </c>
+      <c r="D16" t="str">
+        <f>IF(test1!$C16=$D$4,test1!$D16,"")</f>
+        <v/>
+      </c>
+      <c r="E16" t="str">
+        <f>IF(test1!$C16=$D$4,test1!$E16,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="str">
+        <f>IF(test1!$C17=$A$4,test1!$D17,"")</f>
+        <v/>
+      </c>
+      <c r="B17" t="str">
+        <f>IF(test1!$C17=$A$4,test1!$E17,"")</f>
+        <v/>
+      </c>
+      <c r="D17" t="str">
+        <f>IF(test1!$C17=$D$4,test1!$D17,"")</f>
+        <v/>
+      </c>
+      <c r="E17" t="str">
+        <f>IF(test1!$C17=$D$4,test1!$E17,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="str">
+        <f>IF(test1!$C18=$A$4,test1!$D18,"")</f>
+        <v/>
+      </c>
+      <c r="B18" t="str">
+        <f>IF(test1!$C18=$A$4,test1!$E18,"")</f>
+        <v/>
+      </c>
+      <c r="D18" t="str">
+        <f>IF(test1!$C18=$D$4,test1!$D18,"")</f>
+        <v/>
+      </c>
+      <c r="E18" t="str">
+        <f>IF(test1!$C18=$D$4,test1!$E18,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="str">
+        <f>IF(test1!$C19=$A$4,test1!$D19,"")</f>
+        <v/>
+      </c>
+      <c r="B19" t="str">
+        <f>IF(test1!$C19=$A$4,test1!$E19,"")</f>
+        <v/>
+      </c>
+      <c r="D19" t="str">
+        <f>IF(test1!$C19=$D$4,test1!$D19,"")</f>
+        <v/>
+      </c>
+      <c r="E19" t="str">
+        <f>IF(test1!$C19=$D$4,test1!$E19,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="str">
+        <f>IF(test1!$C20=$A$4,test1!$D20,"")</f>
+        <v/>
+      </c>
+      <c r="B20" t="str">
+        <f>IF(test1!$C20=$A$4,test1!$E20,"")</f>
+        <v/>
+      </c>
+      <c r="D20" t="str">
+        <f>IF(test1!$C20=$D$4,test1!$D20,"")</f>
+        <v/>
+      </c>
+      <c r="E20" t="str">
+        <f>IF(test1!$C20=$D$4,test1!$E20,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="str">
+        <f>IF(test1!$C21=$A$4,test1!$D21,"")</f>
+        <v/>
+      </c>
+      <c r="B21" t="str">
+        <f>IF(test1!$C21=$A$4,test1!$E21,"")</f>
+        <v/>
+      </c>
+      <c r="D21" t="str">
+        <f>IF(test1!$C21=$D$4,test1!$D21,"")</f>
+        <v/>
+      </c>
+      <c r="E21" t="str">
+        <f>IF(test1!$C21=$D$4,test1!$E21,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="str">
+        <f>IF(test1!$C22=$A$4,test1!$D22,"")</f>
+        <v/>
+      </c>
+      <c r="B22" t="str">
+        <f>IF(test1!$C22=$A$4,test1!$E22,"")</f>
+        <v/>
+      </c>
+      <c r="D22" t="str">
+        <f>IF(test1!$C22=$D$4,test1!$D22,"")</f>
+        <v/>
+      </c>
+      <c r="E22" t="str">
+        <f>IF(test1!$C22=$D$4,test1!$E22,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="str">
+        <f>IF(test1!$C23=$A$4,test1!$D23,"")</f>
+        <v/>
+      </c>
+      <c r="B23" t="str">
+        <f>IF(test1!$C23=$A$4,test1!$E23,"")</f>
+        <v/>
+      </c>
+      <c r="D23" t="str">
+        <f>IF(test1!$C23=$D$4,test1!$D23,"")</f>
+        <v/>
+      </c>
+      <c r="E23" t="str">
+        <f>IF(test1!$C23=$D$4,test1!$E23,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="str">
+        <f>IF(test1!$C24=$A$4,test1!$D24,"")</f>
+        <v/>
+      </c>
+      <c r="B24" t="str">
+        <f>IF(test1!$C24=$A$4,test1!$E24,"")</f>
+        <v/>
+      </c>
+      <c r="D24" t="str">
+        <f>IF(test1!$C24=$D$4,test1!$D24,"")</f>
+        <v/>
+      </c>
+      <c r="E24" t="str">
+        <f>IF(test1!$C24=$D$4,test1!$E24,"")</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Created latrun vs latrun test to be able to optimizations on game actionslist
</commit_message>
<xml_diff>
--- a/src/test_results.xlsx
+++ b/src/test_results.xlsx
@@ -1,25 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14895" windowHeight="7875"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7875" windowWidth="14895" xWindow="360" yWindow="300"/>
   </bookViews>
   <sheets>
-    <sheet name="test1" sheetId="1" r:id="rId1"/>
-    <sheet name="compare1" sheetId="2" r:id="rId2"/>
-    <sheet name="Ark3" sheetId="3" r:id="rId3"/>
+    <sheet name="test1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="compare1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Ark3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">test1!$A$5:$E$5</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'test1'!$A$5:$E$5</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t>Time begin</t>
   </si>
@@ -36,10 +35,49 @@
     <t>Time taken to play out game</t>
   </si>
   <si>
+    <t>2019-02-05 00:39:33</t>
+  </si>
+  <si>
+    <t>Skylake-PC</t>
+  </si>
+  <si>
     <t>Latrunculi</t>
   </si>
   <si>
     <t>Latrunculi_ne</t>
+  </si>
+  <si>
+    <t>2019-02-05 00:39:40</t>
+  </si>
+  <si>
+    <t>2019-02-05 00:39:47</t>
+  </si>
+  <si>
+    <t>2019-02-05 00:39:48</t>
+  </si>
+  <si>
+    <t>2019-02-05 00:39:54</t>
+  </si>
+  <si>
+    <t>2019-02-05 00:40:01</t>
+  </si>
+  <si>
+    <t>2019-02-05 00:40:07</t>
+  </si>
+  <si>
+    <t>2019-02-05 00:40:14</t>
+  </si>
+  <si>
+    <t>2019-02-05 00:40:20</t>
+  </si>
+  <si>
+    <t>2019-02-05 00:40:21</t>
+  </si>
+  <si>
+    <t>2019-02-05 00:40:28</t>
+  </si>
+  <si>
+    <t>2019-02-05 00:40:34</t>
   </si>
   <si>
     <t>Time</t>
@@ -49,33 +87,34 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -120,21 +159,20 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Input" xfId="1" builtinId="20"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="20" name="Input" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -422,20 +460,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A5:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A5:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="A6" sqref="A6:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="16.7109375" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="18.28515625"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" width="26.5703125"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:5" s="1" customFormat="1">
+    <row customFormat="1" r="5" s="1" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -452,406 +494,756 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="n">
+        <v>8835</v>
+      </c>
+      <c r="E6" t="n">
+        <v>6.333134412765503</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="n">
+        <v>9485</v>
+      </c>
+      <c r="E7" t="n">
+        <v>6.7969970703125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="n">
+        <v>8835</v>
+      </c>
+      <c r="E8" t="n">
+        <v>6.575448513031006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="n">
+        <v>9485</v>
+      </c>
+      <c r="E9" t="n">
+        <v>6.874972105026245</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="n">
+        <v>8835</v>
+      </c>
+      <c r="E10" t="n">
+        <v>7.012654781341553</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="n">
+        <v>9485</v>
+      </c>
+      <c r="E11" t="n">
+        <v>7.249776363372803</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="n">
+        <v>8835</v>
+      </c>
+      <c r="E12" t="n">
+        <v>6.364303588867188</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="n">
+        <v>9485</v>
+      </c>
+      <c r="E13" t="n">
+        <v>6.56326150894165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="n">
+        <v>8835</v>
+      </c>
+      <c r="E14" t="n">
+        <v>6.528290748596191</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="n">
+        <v>9485</v>
+      </c>
+      <c r="E15" t="n">
+        <v>6.755731582641602</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="n">
+        <v>8835</v>
+      </c>
+      <c r="E16" t="n">
+        <v>6.265946865081787</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="n">
+        <v>9485</v>
+      </c>
+      <c r="E17" t="n">
+        <v>6.501724481582642</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="n">
+        <v>8835</v>
+      </c>
+      <c r="E18" t="n">
+        <v>6.161772966384888</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="n">
+        <v>9485</v>
+      </c>
+      <c r="E19" t="n">
+        <v>6.35172438621521</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="n">
+        <v>8835</v>
+      </c>
+      <c r="E20" t="n">
+        <v>6.568546772003174</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" t="n">
+        <v>9485</v>
+      </c>
+      <c r="E21" t="n">
+        <v>6.792579650878906</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="n">
+        <v>8835</v>
+      </c>
+      <c r="E22" t="n">
+        <v>6.901476621627808</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="n">
+        <v>9485</v>
+      </c>
+      <c r="E23" t="n">
+        <v>7.108088731765747</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" t="n">
+        <v>8835</v>
+      </c>
+      <c r="E24" t="n">
+        <v>6.386498928070068</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" t="n">
+        <v>9485</v>
+      </c>
+      <c r="E25" t="n">
+        <v>6.669204473495483</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A5:E5"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A4:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="9.7109375"/>
+    <col customWidth="1" max="4" min="4" width="13.85546875"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="15.75" r="5" s="3" spans="1:5" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" t="str">
+      <c r="A6">
         <f>IF(test1!$C6=$A$4,test1!$D6,"")</f>
         <v/>
       </c>
-      <c r="B6" t="str">
+      <c r="B6">
         <f>IF(test1!$C6=$A$4,test1!$E6,"")</f>
         <v/>
       </c>
-      <c r="D6" t="str">
+      <c r="D6">
         <f>IF(test1!$C6=$D$4,test1!$D6,"")</f>
         <v/>
       </c>
-      <c r="E6" t="str">
+      <c r="E6">
         <f>IF(test1!$C6=$D$4,test1!$E6,"")</f>
         <v/>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" t="str">
+      <c r="A7">
         <f>IF(test1!$C7=$A$4,test1!$D7,"")</f>
         <v/>
       </c>
-      <c r="B7" t="str">
+      <c r="B7">
         <f>IF(test1!$C7=$A$4,test1!$E7,"")</f>
         <v/>
       </c>
-      <c r="D7" t="str">
+      <c r="D7">
         <f>IF(test1!$C7=$D$4,test1!$D7,"")</f>
         <v/>
       </c>
-      <c r="E7" t="str">
+      <c r="E7">
         <f>IF(test1!$C7=$D$4,test1!$E7,"")</f>
         <v/>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" t="str">
+      <c r="A8">
         <f>IF(test1!$C8=$A$4,test1!$D8,"")</f>
         <v/>
       </c>
-      <c r="B8" t="str">
+      <c r="B8">
         <f>IF(test1!$C8=$A$4,test1!$E8,"")</f>
         <v/>
       </c>
-      <c r="D8" t="str">
+      <c r="D8">
         <f>IF(test1!$C8=$D$4,test1!$D8,"")</f>
         <v/>
       </c>
-      <c r="E8" t="str">
+      <c r="E8">
         <f>IF(test1!$C8=$D$4,test1!$E8,"")</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" t="str">
+      <c r="A9">
         <f>IF(test1!$C9=$A$4,test1!$D9,"")</f>
         <v/>
       </c>
-      <c r="B9" t="str">
+      <c r="B9">
         <f>IF(test1!$C9=$A$4,test1!$E9,"")</f>
         <v/>
       </c>
-      <c r="D9" t="str">
+      <c r="D9">
         <f>IF(test1!$C9=$D$4,test1!$D9,"")</f>
         <v/>
       </c>
-      <c r="E9" t="str">
+      <c r="E9">
         <f>IF(test1!$C9=$D$4,test1!$E9,"")</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" t="str">
+      <c r="A10">
         <f>IF(test1!$C10=$A$4,test1!$D10,"")</f>
         <v/>
       </c>
-      <c r="B10" t="str">
+      <c r="B10">
         <f>IF(test1!$C10=$A$4,test1!$E10,"")</f>
         <v/>
       </c>
-      <c r="D10" t="str">
+      <c r="D10">
         <f>IF(test1!$C10=$D$4,test1!$D10,"")</f>
         <v/>
       </c>
-      <c r="E10" t="str">
+      <c r="E10">
         <f>IF(test1!$C10=$D$4,test1!$E10,"")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" t="str">
+      <c r="A11">
         <f>IF(test1!$C11=$A$4,test1!$D11,"")</f>
         <v/>
       </c>
-      <c r="B11" t="str">
+      <c r="B11">
         <f>IF(test1!$C11=$A$4,test1!$E11,"")</f>
         <v/>
       </c>
-      <c r="D11" t="str">
+      <c r="D11">
         <f>IF(test1!$C11=$D$4,test1!$D11,"")</f>
         <v/>
       </c>
-      <c r="E11" t="str">
+      <c r="E11">
         <f>IF(test1!$C11=$D$4,test1!$E11,"")</f>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" t="str">
+      <c r="A12">
         <f>IF(test1!$C12=$A$4,test1!$D12,"")</f>
         <v/>
       </c>
-      <c r="B12" t="str">
+      <c r="B12">
         <f>IF(test1!$C12=$A$4,test1!$E12,"")</f>
         <v/>
       </c>
-      <c r="D12" t="str">
+      <c r="D12">
         <f>IF(test1!$C12=$D$4,test1!$D12,"")</f>
         <v/>
       </c>
-      <c r="E12" t="str">
+      <c r="E12">
         <f>IF(test1!$C12=$D$4,test1!$E12,"")</f>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" t="str">
+      <c r="A13">
         <f>IF(test1!$C13=$A$4,test1!$D13,"")</f>
         <v/>
       </c>
-      <c r="B13" t="str">
+      <c r="B13">
         <f>IF(test1!$C13=$A$4,test1!$E13,"")</f>
         <v/>
       </c>
-      <c r="D13" t="str">
+      <c r="D13">
         <f>IF(test1!$C13=$D$4,test1!$D13,"")</f>
         <v/>
       </c>
-      <c r="E13" t="str">
+      <c r="E13">
         <f>IF(test1!$C13=$D$4,test1!$E13,"")</f>
         <v/>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" t="str">
+      <c r="A14">
         <f>IF(test1!$C14=$A$4,test1!$D14,"")</f>
         <v/>
       </c>
-      <c r="B14" t="str">
+      <c r="B14">
         <f>IF(test1!$C14=$A$4,test1!$E14,"")</f>
         <v/>
       </c>
-      <c r="D14" t="str">
+      <c r="D14">
         <f>IF(test1!$C14=$D$4,test1!$D14,"")</f>
         <v/>
       </c>
-      <c r="E14" t="str">
+      <c r="E14">
         <f>IF(test1!$C14=$D$4,test1!$E14,"")</f>
         <v/>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" t="str">
+      <c r="A15">
         <f>IF(test1!$C15=$A$4,test1!$D15,"")</f>
         <v/>
       </c>
-      <c r="B15" t="str">
+      <c r="B15">
         <f>IF(test1!$C15=$A$4,test1!$E15,"")</f>
         <v/>
       </c>
-      <c r="D15" t="str">
+      <c r="D15">
         <f>IF(test1!$C15=$D$4,test1!$D15,"")</f>
         <v/>
       </c>
-      <c r="E15" t="str">
+      <c r="E15">
         <f>IF(test1!$C15=$D$4,test1!$E15,"")</f>
         <v/>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" t="str">
+      <c r="A16">
         <f>IF(test1!$C16=$A$4,test1!$D16,"")</f>
         <v/>
       </c>
-      <c r="B16" t="str">
+      <c r="B16">
         <f>IF(test1!$C16=$A$4,test1!$E16,"")</f>
         <v/>
       </c>
-      <c r="D16" t="str">
+      <c r="D16">
         <f>IF(test1!$C16=$D$4,test1!$D16,"")</f>
         <v/>
       </c>
-      <c r="E16" t="str">
+      <c r="E16">
         <f>IF(test1!$C16=$D$4,test1!$E16,"")</f>
         <v/>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" t="str">
+      <c r="A17">
         <f>IF(test1!$C17=$A$4,test1!$D17,"")</f>
         <v/>
       </c>
-      <c r="B17" t="str">
+      <c r="B17">
         <f>IF(test1!$C17=$A$4,test1!$E17,"")</f>
         <v/>
       </c>
-      <c r="D17" t="str">
+      <c r="D17">
         <f>IF(test1!$C17=$D$4,test1!$D17,"")</f>
         <v/>
       </c>
-      <c r="E17" t="str">
+      <c r="E17">
         <f>IF(test1!$C17=$D$4,test1!$E17,"")</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" t="str">
+      <c r="A18">
         <f>IF(test1!$C18=$A$4,test1!$D18,"")</f>
         <v/>
       </c>
-      <c r="B18" t="str">
+      <c r="B18">
         <f>IF(test1!$C18=$A$4,test1!$E18,"")</f>
         <v/>
       </c>
-      <c r="D18" t="str">
+      <c r="D18">
         <f>IF(test1!$C18=$D$4,test1!$D18,"")</f>
         <v/>
       </c>
-      <c r="E18" t="str">
+      <c r="E18">
         <f>IF(test1!$C18=$D$4,test1!$E18,"")</f>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" t="str">
+      <c r="A19">
         <f>IF(test1!$C19=$A$4,test1!$D19,"")</f>
         <v/>
       </c>
-      <c r="B19" t="str">
+      <c r="B19">
         <f>IF(test1!$C19=$A$4,test1!$E19,"")</f>
         <v/>
       </c>
-      <c r="D19" t="str">
+      <c r="D19">
         <f>IF(test1!$C19=$D$4,test1!$D19,"")</f>
         <v/>
       </c>
-      <c r="E19" t="str">
+      <c r="E19">
         <f>IF(test1!$C19=$D$4,test1!$E19,"")</f>
         <v/>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" t="str">
+      <c r="A20">
         <f>IF(test1!$C20=$A$4,test1!$D20,"")</f>
         <v/>
       </c>
-      <c r="B20" t="str">
+      <c r="B20">
         <f>IF(test1!$C20=$A$4,test1!$E20,"")</f>
         <v/>
       </c>
-      <c r="D20" t="str">
+      <c r="D20">
         <f>IF(test1!$C20=$D$4,test1!$D20,"")</f>
         <v/>
       </c>
-      <c r="E20" t="str">
+      <c r="E20">
         <f>IF(test1!$C20=$D$4,test1!$E20,"")</f>
         <v/>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" t="str">
+      <c r="A21">
         <f>IF(test1!$C21=$A$4,test1!$D21,"")</f>
         <v/>
       </c>
-      <c r="B21" t="str">
+      <c r="B21">
         <f>IF(test1!$C21=$A$4,test1!$E21,"")</f>
         <v/>
       </c>
-      <c r="D21" t="str">
+      <c r="D21">
         <f>IF(test1!$C21=$D$4,test1!$D21,"")</f>
         <v/>
       </c>
-      <c r="E21" t="str">
+      <c r="E21">
         <f>IF(test1!$C21=$D$4,test1!$E21,"")</f>
         <v/>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" t="str">
+      <c r="A22">
         <f>IF(test1!$C22=$A$4,test1!$D22,"")</f>
         <v/>
       </c>
-      <c r="B22" t="str">
+      <c r="B22">
         <f>IF(test1!$C22=$A$4,test1!$E22,"")</f>
         <v/>
       </c>
-      <c r="D22" t="str">
+      <c r="D22">
         <f>IF(test1!$C22=$D$4,test1!$D22,"")</f>
         <v/>
       </c>
-      <c r="E22" t="str">
+      <c r="E22">
         <f>IF(test1!$C22=$D$4,test1!$E22,"")</f>
         <v/>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" t="str">
+      <c r="A23">
         <f>IF(test1!$C23=$A$4,test1!$D23,"")</f>
         <v/>
       </c>
-      <c r="B23" t="str">
+      <c r="B23">
         <f>IF(test1!$C23=$A$4,test1!$E23,"")</f>
         <v/>
       </c>
-      <c r="D23" t="str">
+      <c r="D23">
         <f>IF(test1!$C23=$D$4,test1!$D23,"")</f>
         <v/>
       </c>
-      <c r="E23" t="str">
+      <c r="E23">
         <f>IF(test1!$C23=$D$4,test1!$E23,"")</f>
         <v/>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" t="str">
+      <c r="A24">
         <f>IF(test1!$C24=$A$4,test1!$D24,"")</f>
         <v/>
       </c>
-      <c r="B24" t="str">
+      <c r="B24">
         <f>IF(test1!$C24=$A$4,test1!$E24,"")</f>
         <v/>
       </c>
-      <c r="D24" t="str">
+      <c r="D24">
         <f>IF(test1!$C24=$D$4,test1!$D24,"")</f>
         <v/>
       </c>
-      <c r="E24" t="str">
+      <c r="E24">
         <f>IF(test1!$C24=$D$4,test1!$E24,"")</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup copies="0" horizontalDpi="0" orientation="portrait" paperSize="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Done for tonight, backup
</commit_message>
<xml_diff>
--- a/src/test_results.xlsx
+++ b/src/test_results.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7875" windowWidth="14895" xWindow="360" yWindow="300"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="14895" windowHeight="7875"/>
   </bookViews>
   <sheets>
-    <sheet name="test1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="compare1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Ark3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="test1" sheetId="1" r:id="rId1"/>
+    <sheet name="compare1" sheetId="2" r:id="rId2"/>
+    <sheet name="Ark3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'test1'!$A$5:$E$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">test1!$A$5:$E$5</definedName>
   </definedNames>
-  <calcPr calcId="125725" fullCalcOnLoad="1"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>Time begin</t>
   </si>
@@ -35,49 +36,10 @@
     <t>Time taken to play out game</t>
   </si>
   <si>
-    <t>2019-02-05 00:39:33</t>
-  </si>
-  <si>
-    <t>Skylake-PC</t>
-  </si>
-  <si>
     <t>Latrunculi</t>
   </si>
   <si>
     <t>Latrunculi_ne</t>
-  </si>
-  <si>
-    <t>2019-02-05 00:39:40</t>
-  </si>
-  <si>
-    <t>2019-02-05 00:39:47</t>
-  </si>
-  <si>
-    <t>2019-02-05 00:39:48</t>
-  </si>
-  <si>
-    <t>2019-02-05 00:39:54</t>
-  </si>
-  <si>
-    <t>2019-02-05 00:40:01</t>
-  </si>
-  <si>
-    <t>2019-02-05 00:40:07</t>
-  </si>
-  <si>
-    <t>2019-02-05 00:40:14</t>
-  </si>
-  <si>
-    <t>2019-02-05 00:40:20</t>
-  </si>
-  <si>
-    <t>2019-02-05 00:40:21</t>
-  </si>
-  <si>
-    <t>2019-02-05 00:40:28</t>
-  </si>
-  <si>
-    <t>2019-02-05 00:40:34</t>
   </si>
   <si>
     <t>Time</t>
@@ -87,34 +49,33 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF3F3F76"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -159,20 +120,21 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="20" name="Input" xfId="1"/>
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -460,24 +422,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A5:E25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A5:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD7"/>
+      <selection activeCell="A6" sqref="A6:XFD37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="16.7109375" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="18.28515625"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" width="26.5703125"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="5" s="1" spans="1:5">
+    <row r="5" spans="1:5" s="1" customFormat="1">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,756 +452,406 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="n">
-        <v>8835</v>
-      </c>
-      <c r="E6" t="n">
-        <v>6.333134412765503</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="n">
-        <v>9485</v>
-      </c>
-      <c r="E7" t="n">
-        <v>6.7969970703125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="n">
-        <v>8835</v>
-      </c>
-      <c r="E8" t="n">
-        <v>6.575448513031006</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="n">
-        <v>9485</v>
-      </c>
-      <c r="E9" t="n">
-        <v>6.874972105026245</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="n">
-        <v>8835</v>
-      </c>
-      <c r="E10" t="n">
-        <v>7.012654781341553</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="n">
-        <v>9485</v>
-      </c>
-      <c r="E11" t="n">
-        <v>7.249776363372803</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" t="n">
-        <v>8835</v>
-      </c>
-      <c r="E12" t="n">
-        <v>6.364303588867188</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" t="n">
-        <v>9485</v>
-      </c>
-      <c r="E13" t="n">
-        <v>6.56326150894165</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" t="n">
-        <v>8835</v>
-      </c>
-      <c r="E14" t="n">
-        <v>6.528290748596191</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" t="n">
-        <v>9485</v>
-      </c>
-      <c r="E15" t="n">
-        <v>6.755731582641602</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" t="n">
-        <v>8835</v>
-      </c>
-      <c r="E16" t="n">
-        <v>6.265946865081787</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" t="n">
-        <v>9485</v>
-      </c>
-      <c r="E17" t="n">
-        <v>6.501724481582642</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" t="n">
-        <v>8835</v>
-      </c>
-      <c r="E18" t="n">
-        <v>6.161772966384888</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" t="n">
-        <v>9485</v>
-      </c>
-      <c r="E19" t="n">
-        <v>6.35172438621521</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" t="n">
-        <v>8835</v>
-      </c>
-      <c r="E20" t="n">
-        <v>6.568546772003174</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" t="n">
-        <v>9485</v>
-      </c>
-      <c r="E21" t="n">
-        <v>6.792579650878906</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" t="n">
-        <v>8835</v>
-      </c>
-      <c r="E22" t="n">
-        <v>6.901476621627808</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" t="n">
-        <v>9485</v>
-      </c>
-      <c r="E23" t="n">
-        <v>7.108088731765747</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" t="n">
-        <v>8835</v>
-      </c>
-      <c r="E24" t="n">
-        <v>6.386498928070068</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" t="n">
-        <v>9485</v>
-      </c>
-      <c r="E25" t="n">
-        <v>6.669204473495483</v>
-      </c>
-    </row>
   </sheetData>
   <autoFilter ref="A5:E5"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="9.7109375"/>
-    <col customWidth="1" max="4" min="4" width="13.85546875"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="15.75" r="5" s="3" spans="1:5" thickBot="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6">
+      <c r="A6" t="str">
         <f>IF(test1!$C6=$A$4,test1!$D6,"")</f>
         <v/>
       </c>
-      <c r="B6">
+      <c r="B6" t="str">
         <f>IF(test1!$C6=$A$4,test1!$E6,"")</f>
         <v/>
       </c>
-      <c r="D6">
+      <c r="D6" t="str">
         <f>IF(test1!$C6=$D$4,test1!$D6,"")</f>
         <v/>
       </c>
-      <c r="E6">
+      <c r="E6" t="str">
         <f>IF(test1!$C6=$D$4,test1!$E6,"")</f>
         <v/>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7">
+      <c r="A7" t="str">
         <f>IF(test1!$C7=$A$4,test1!$D7,"")</f>
         <v/>
       </c>
-      <c r="B7">
+      <c r="B7" t="str">
         <f>IF(test1!$C7=$A$4,test1!$E7,"")</f>
         <v/>
       </c>
-      <c r="D7">
+      <c r="D7" t="str">
         <f>IF(test1!$C7=$D$4,test1!$D7,"")</f>
         <v/>
       </c>
-      <c r="E7">
+      <c r="E7" t="str">
         <f>IF(test1!$C7=$D$4,test1!$E7,"")</f>
         <v/>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8">
+      <c r="A8" t="str">
         <f>IF(test1!$C8=$A$4,test1!$D8,"")</f>
         <v/>
       </c>
-      <c r="B8">
+      <c r="B8" t="str">
         <f>IF(test1!$C8=$A$4,test1!$E8,"")</f>
         <v/>
       </c>
-      <c r="D8">
+      <c r="D8" t="str">
         <f>IF(test1!$C8=$D$4,test1!$D8,"")</f>
         <v/>
       </c>
-      <c r="E8">
+      <c r="E8" t="str">
         <f>IF(test1!$C8=$D$4,test1!$E8,"")</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9">
+      <c r="A9" t="str">
         <f>IF(test1!$C9=$A$4,test1!$D9,"")</f>
         <v/>
       </c>
-      <c r="B9">
+      <c r="B9" t="str">
         <f>IF(test1!$C9=$A$4,test1!$E9,"")</f>
         <v/>
       </c>
-      <c r="D9">
+      <c r="D9" t="str">
         <f>IF(test1!$C9=$D$4,test1!$D9,"")</f>
         <v/>
       </c>
-      <c r="E9">
+      <c r="E9" t="str">
         <f>IF(test1!$C9=$D$4,test1!$E9,"")</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10">
+      <c r="A10" t="str">
         <f>IF(test1!$C10=$A$4,test1!$D10,"")</f>
         <v/>
       </c>
-      <c r="B10">
+      <c r="B10" t="str">
         <f>IF(test1!$C10=$A$4,test1!$E10,"")</f>
         <v/>
       </c>
-      <c r="D10">
+      <c r="D10" t="str">
         <f>IF(test1!$C10=$D$4,test1!$D10,"")</f>
         <v/>
       </c>
-      <c r="E10">
+      <c r="E10" t="str">
         <f>IF(test1!$C10=$D$4,test1!$E10,"")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11">
+      <c r="A11" t="str">
         <f>IF(test1!$C11=$A$4,test1!$D11,"")</f>
         <v/>
       </c>
-      <c r="B11">
+      <c r="B11" t="str">
         <f>IF(test1!$C11=$A$4,test1!$E11,"")</f>
         <v/>
       </c>
-      <c r="D11">
+      <c r="D11" t="str">
         <f>IF(test1!$C11=$D$4,test1!$D11,"")</f>
         <v/>
       </c>
-      <c r="E11">
+      <c r="E11" t="str">
         <f>IF(test1!$C11=$D$4,test1!$E11,"")</f>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12">
+      <c r="A12" t="str">
         <f>IF(test1!$C12=$A$4,test1!$D12,"")</f>
         <v/>
       </c>
-      <c r="B12">
+      <c r="B12" t="str">
         <f>IF(test1!$C12=$A$4,test1!$E12,"")</f>
         <v/>
       </c>
-      <c r="D12">
+      <c r="D12" t="str">
         <f>IF(test1!$C12=$D$4,test1!$D12,"")</f>
         <v/>
       </c>
-      <c r="E12">
+      <c r="E12" t="str">
         <f>IF(test1!$C12=$D$4,test1!$E12,"")</f>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13">
+      <c r="A13" t="str">
         <f>IF(test1!$C13=$A$4,test1!$D13,"")</f>
         <v/>
       </c>
-      <c r="B13">
+      <c r="B13" t="str">
         <f>IF(test1!$C13=$A$4,test1!$E13,"")</f>
         <v/>
       </c>
-      <c r="D13">
+      <c r="D13" t="str">
         <f>IF(test1!$C13=$D$4,test1!$D13,"")</f>
         <v/>
       </c>
-      <c r="E13">
+      <c r="E13" t="str">
         <f>IF(test1!$C13=$D$4,test1!$E13,"")</f>
         <v/>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14">
+      <c r="A14" t="str">
         <f>IF(test1!$C14=$A$4,test1!$D14,"")</f>
         <v/>
       </c>
-      <c r="B14">
+      <c r="B14" t="str">
         <f>IF(test1!$C14=$A$4,test1!$E14,"")</f>
         <v/>
       </c>
-      <c r="D14">
+      <c r="D14" t="str">
         <f>IF(test1!$C14=$D$4,test1!$D14,"")</f>
         <v/>
       </c>
-      <c r="E14">
+      <c r="E14" t="str">
         <f>IF(test1!$C14=$D$4,test1!$E14,"")</f>
         <v/>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15">
+      <c r="A15" t="str">
         <f>IF(test1!$C15=$A$4,test1!$D15,"")</f>
         <v/>
       </c>
-      <c r="B15">
+      <c r="B15" t="str">
         <f>IF(test1!$C15=$A$4,test1!$E15,"")</f>
         <v/>
       </c>
-      <c r="D15">
+      <c r="D15" t="str">
         <f>IF(test1!$C15=$D$4,test1!$D15,"")</f>
         <v/>
       </c>
-      <c r="E15">
+      <c r="E15" t="str">
         <f>IF(test1!$C15=$D$4,test1!$E15,"")</f>
         <v/>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16">
+      <c r="A16" t="str">
         <f>IF(test1!$C16=$A$4,test1!$D16,"")</f>
         <v/>
       </c>
-      <c r="B16">
+      <c r="B16" t="str">
         <f>IF(test1!$C16=$A$4,test1!$E16,"")</f>
         <v/>
       </c>
-      <c r="D16">
+      <c r="D16" t="str">
         <f>IF(test1!$C16=$D$4,test1!$D16,"")</f>
         <v/>
       </c>
-      <c r="E16">
+      <c r="E16" t="str">
         <f>IF(test1!$C16=$D$4,test1!$E16,"")</f>
         <v/>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17">
+      <c r="A17" t="str">
         <f>IF(test1!$C17=$A$4,test1!$D17,"")</f>
         <v/>
       </c>
-      <c r="B17">
+      <c r="B17" t="str">
         <f>IF(test1!$C17=$A$4,test1!$E17,"")</f>
         <v/>
       </c>
-      <c r="D17">
+      <c r="D17" t="str">
         <f>IF(test1!$C17=$D$4,test1!$D17,"")</f>
         <v/>
       </c>
-      <c r="E17">
+      <c r="E17" t="str">
         <f>IF(test1!$C17=$D$4,test1!$E17,"")</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18">
+      <c r="A18" t="str">
         <f>IF(test1!$C18=$A$4,test1!$D18,"")</f>
         <v/>
       </c>
-      <c r="B18">
+      <c r="B18" t="str">
         <f>IF(test1!$C18=$A$4,test1!$E18,"")</f>
         <v/>
       </c>
-      <c r="D18">
+      <c r="D18" t="str">
         <f>IF(test1!$C18=$D$4,test1!$D18,"")</f>
         <v/>
       </c>
-      <c r="E18">
+      <c r="E18" t="str">
         <f>IF(test1!$C18=$D$4,test1!$E18,"")</f>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19">
+      <c r="A19" t="str">
         <f>IF(test1!$C19=$A$4,test1!$D19,"")</f>
         <v/>
       </c>
-      <c r="B19">
+      <c r="B19" t="str">
         <f>IF(test1!$C19=$A$4,test1!$E19,"")</f>
         <v/>
       </c>
-      <c r="D19">
+      <c r="D19" t="str">
         <f>IF(test1!$C19=$D$4,test1!$D19,"")</f>
         <v/>
       </c>
-      <c r="E19">
+      <c r="E19" t="str">
         <f>IF(test1!$C19=$D$4,test1!$E19,"")</f>
         <v/>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20">
+      <c r="A20" t="str">
         <f>IF(test1!$C20=$A$4,test1!$D20,"")</f>
         <v/>
       </c>
-      <c r="B20">
+      <c r="B20" t="str">
         <f>IF(test1!$C20=$A$4,test1!$E20,"")</f>
         <v/>
       </c>
-      <c r="D20">
+      <c r="D20" t="str">
         <f>IF(test1!$C20=$D$4,test1!$D20,"")</f>
         <v/>
       </c>
-      <c r="E20">
+      <c r="E20" t="str">
         <f>IF(test1!$C20=$D$4,test1!$E20,"")</f>
         <v/>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21">
+      <c r="A21" t="str">
         <f>IF(test1!$C21=$A$4,test1!$D21,"")</f>
         <v/>
       </c>
-      <c r="B21">
+      <c r="B21" t="str">
         <f>IF(test1!$C21=$A$4,test1!$E21,"")</f>
         <v/>
       </c>
-      <c r="D21">
+      <c r="D21" t="str">
         <f>IF(test1!$C21=$D$4,test1!$D21,"")</f>
         <v/>
       </c>
-      <c r="E21">
+      <c r="E21" t="str">
         <f>IF(test1!$C21=$D$4,test1!$E21,"")</f>
         <v/>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22">
+      <c r="A22" t="str">
         <f>IF(test1!$C22=$A$4,test1!$D22,"")</f>
         <v/>
       </c>
-      <c r="B22">
+      <c r="B22" t="str">
         <f>IF(test1!$C22=$A$4,test1!$E22,"")</f>
         <v/>
       </c>
-      <c r="D22">
+      <c r="D22" t="str">
         <f>IF(test1!$C22=$D$4,test1!$D22,"")</f>
         <v/>
       </c>
-      <c r="E22">
+      <c r="E22" t="str">
         <f>IF(test1!$C22=$D$4,test1!$E22,"")</f>
         <v/>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23">
+      <c r="A23" t="str">
         <f>IF(test1!$C23=$A$4,test1!$D23,"")</f>
         <v/>
       </c>
-      <c r="B23">
+      <c r="B23" t="str">
         <f>IF(test1!$C23=$A$4,test1!$E23,"")</f>
         <v/>
       </c>
-      <c r="D23">
+      <c r="D23" t="str">
         <f>IF(test1!$C23=$D$4,test1!$D23,"")</f>
         <v/>
       </c>
-      <c r="E23">
+      <c r="E23" t="str">
         <f>IF(test1!$C23=$D$4,test1!$E23,"")</f>
         <v/>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24">
+      <c r="A24" t="str">
         <f>IF(test1!$C24=$A$4,test1!$D24,"")</f>
         <v/>
       </c>
-      <c r="B24">
+      <c r="B24" t="str">
         <f>IF(test1!$C24=$A$4,test1!$E24,"")</f>
         <v/>
       </c>
-      <c r="D24">
+      <c r="D24" t="str">
         <f>IF(test1!$C24=$D$4,test1!$D24,"")</f>
         <v/>
       </c>
-      <c r="E24">
+      <c r="E24" t="str">
         <f>IF(test1!$C24=$D$4,test1!$E24,"")</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup copies="0" horizontalDpi="0" orientation="portrait" paperSize="0" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Before pull from dev
</commit_message>
<xml_diff>
--- a/src/test_results.xlsx
+++ b/src/test_results.xlsx
@@ -36,10 +36,10 @@
     <t>Time taken to play out game</t>
   </si>
   <si>
-    <t>Latrunculi</t>
+    <t>Latrunculi_ne</t>
   </si>
   <si>
-    <t>Latrunculi_ne</t>
+    <t>Latrunculi</t>
   </si>
   <si>
     <t>Time</t>
@@ -426,7 +426,7 @@
   <dimension ref="A5:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD37"/>
+      <selection activeCell="A6" sqref="A6:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15"/>
@@ -475,10 +475,10 @@
   <sheetData>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1">

</xml_diff>

<commit_message>
Kinda a added sql loggin to the project..
</commit_message>
<xml_diff>
--- a/src/test_results.xlsx
+++ b/src/test_results.xlsx
@@ -1,25 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14895" windowHeight="7875"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7875" windowWidth="14895" xWindow="360" yWindow="300"/>
   </bookViews>
   <sheets>
-    <sheet name="test1" sheetId="1" r:id="rId1"/>
-    <sheet name="compare1" sheetId="2" r:id="rId2"/>
-    <sheet name="Ark3" sheetId="3" r:id="rId3"/>
+    <sheet name="test1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="compare1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Ark3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">test1!$A$5:$E$5</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'test1'!$A$5:$E$5</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>Time begin</t>
   </si>
@@ -36,7 +35,19 @@
     <t>Time taken to play out game</t>
   </si>
   <si>
+    <t>2019-02-05 19:17:15</t>
+  </si>
+  <si>
+    <t>Skylake-PC</t>
+  </si>
+  <si>
     <t>Latrunculi_ne</t>
+  </si>
+  <si>
+    <t>2019-02-05 19:20:23</t>
+  </si>
+  <si>
+    <t>2019-02-05 19:21:18</t>
   </si>
   <si>
     <t>Latrunculi</t>
@@ -49,33 +60,34 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -120,21 +132,20 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Input" xfId="1" builtinId="20"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="20" name="Input" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -422,20 +433,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A5:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A5:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="16.7109375" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="18.28515625"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" width="26.5703125"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:5" s="1" customFormat="1">
+    <row customFormat="1" r="5" s="1" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -452,406 +467,467 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3668</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1.898438453674316</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="n">
+        <v>6735</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2.942668676376343</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="n">
+        <v>4389</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3.050406694412231</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A5:E5"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A4:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="9.7109375"/>
+    <col customWidth="1" max="4" min="4" width="13.85546875"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="15.75" r="5" s="3" spans="1:5" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" t="str">
+      <c r="A6">
         <f>IF(test1!$C6=$A$4,test1!$D6,"")</f>
         <v/>
       </c>
-      <c r="B6" t="str">
+      <c r="B6">
         <f>IF(test1!$C6=$A$4,test1!$E6,"")</f>
         <v/>
       </c>
-      <c r="D6" t="str">
+      <c r="D6">
         <f>IF(test1!$C6=$D$4,test1!$D6,"")</f>
         <v/>
       </c>
-      <c r="E6" t="str">
+      <c r="E6">
         <f>IF(test1!$C6=$D$4,test1!$E6,"")</f>
         <v/>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" t="str">
+      <c r="A7">
         <f>IF(test1!$C7=$A$4,test1!$D7,"")</f>
         <v/>
       </c>
-      <c r="B7" t="str">
+      <c r="B7">
         <f>IF(test1!$C7=$A$4,test1!$E7,"")</f>
         <v/>
       </c>
-      <c r="D7" t="str">
+      <c r="D7">
         <f>IF(test1!$C7=$D$4,test1!$D7,"")</f>
         <v/>
       </c>
-      <c r="E7" t="str">
+      <c r="E7">
         <f>IF(test1!$C7=$D$4,test1!$E7,"")</f>
         <v/>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" t="str">
+      <c r="A8">
         <f>IF(test1!$C8=$A$4,test1!$D8,"")</f>
         <v/>
       </c>
-      <c r="B8" t="str">
+      <c r="B8">
         <f>IF(test1!$C8=$A$4,test1!$E8,"")</f>
         <v/>
       </c>
-      <c r="D8" t="str">
+      <c r="D8">
         <f>IF(test1!$C8=$D$4,test1!$D8,"")</f>
         <v/>
       </c>
-      <c r="E8" t="str">
+      <c r="E8">
         <f>IF(test1!$C8=$D$4,test1!$E8,"")</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" t="str">
+      <c r="A9">
         <f>IF(test1!$C9=$A$4,test1!$D9,"")</f>
         <v/>
       </c>
-      <c r="B9" t="str">
+      <c r="B9">
         <f>IF(test1!$C9=$A$4,test1!$E9,"")</f>
         <v/>
       </c>
-      <c r="D9" t="str">
+      <c r="D9">
         <f>IF(test1!$C9=$D$4,test1!$D9,"")</f>
         <v/>
       </c>
-      <c r="E9" t="str">
+      <c r="E9">
         <f>IF(test1!$C9=$D$4,test1!$E9,"")</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" t="str">
+      <c r="A10">
         <f>IF(test1!$C10=$A$4,test1!$D10,"")</f>
         <v/>
       </c>
-      <c r="B10" t="str">
+      <c r="B10">
         <f>IF(test1!$C10=$A$4,test1!$E10,"")</f>
         <v/>
       </c>
-      <c r="D10" t="str">
+      <c r="D10">
         <f>IF(test1!$C10=$D$4,test1!$D10,"")</f>
         <v/>
       </c>
-      <c r="E10" t="str">
+      <c r="E10">
         <f>IF(test1!$C10=$D$4,test1!$E10,"")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" t="str">
+      <c r="A11">
         <f>IF(test1!$C11=$A$4,test1!$D11,"")</f>
         <v/>
       </c>
-      <c r="B11" t="str">
+      <c r="B11">
         <f>IF(test1!$C11=$A$4,test1!$E11,"")</f>
         <v/>
       </c>
-      <c r="D11" t="str">
+      <c r="D11">
         <f>IF(test1!$C11=$D$4,test1!$D11,"")</f>
         <v/>
       </c>
-      <c r="E11" t="str">
+      <c r="E11">
         <f>IF(test1!$C11=$D$4,test1!$E11,"")</f>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" t="str">
+      <c r="A12">
         <f>IF(test1!$C12=$A$4,test1!$D12,"")</f>
         <v/>
       </c>
-      <c r="B12" t="str">
+      <c r="B12">
         <f>IF(test1!$C12=$A$4,test1!$E12,"")</f>
         <v/>
       </c>
-      <c r="D12" t="str">
+      <c r="D12">
         <f>IF(test1!$C12=$D$4,test1!$D12,"")</f>
         <v/>
       </c>
-      <c r="E12" t="str">
+      <c r="E12">
         <f>IF(test1!$C12=$D$4,test1!$E12,"")</f>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" t="str">
+      <c r="A13">
         <f>IF(test1!$C13=$A$4,test1!$D13,"")</f>
         <v/>
       </c>
-      <c r="B13" t="str">
+      <c r="B13">
         <f>IF(test1!$C13=$A$4,test1!$E13,"")</f>
         <v/>
       </c>
-      <c r="D13" t="str">
+      <c r="D13">
         <f>IF(test1!$C13=$D$4,test1!$D13,"")</f>
         <v/>
       </c>
-      <c r="E13" t="str">
+      <c r="E13">
         <f>IF(test1!$C13=$D$4,test1!$E13,"")</f>
         <v/>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" t="str">
+      <c r="A14">
         <f>IF(test1!$C14=$A$4,test1!$D14,"")</f>
         <v/>
       </c>
-      <c r="B14" t="str">
+      <c r="B14">
         <f>IF(test1!$C14=$A$4,test1!$E14,"")</f>
         <v/>
       </c>
-      <c r="D14" t="str">
+      <c r="D14">
         <f>IF(test1!$C14=$D$4,test1!$D14,"")</f>
         <v/>
       </c>
-      <c r="E14" t="str">
+      <c r="E14">
         <f>IF(test1!$C14=$D$4,test1!$E14,"")</f>
         <v/>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" t="str">
+      <c r="A15">
         <f>IF(test1!$C15=$A$4,test1!$D15,"")</f>
         <v/>
       </c>
-      <c r="B15" t="str">
+      <c r="B15">
         <f>IF(test1!$C15=$A$4,test1!$E15,"")</f>
         <v/>
       </c>
-      <c r="D15" t="str">
+      <c r="D15">
         <f>IF(test1!$C15=$D$4,test1!$D15,"")</f>
         <v/>
       </c>
-      <c r="E15" t="str">
+      <c r="E15">
         <f>IF(test1!$C15=$D$4,test1!$E15,"")</f>
         <v/>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" t="str">
+      <c r="A16">
         <f>IF(test1!$C16=$A$4,test1!$D16,"")</f>
         <v/>
       </c>
-      <c r="B16" t="str">
+      <c r="B16">
         <f>IF(test1!$C16=$A$4,test1!$E16,"")</f>
         <v/>
       </c>
-      <c r="D16" t="str">
+      <c r="D16">
         <f>IF(test1!$C16=$D$4,test1!$D16,"")</f>
         <v/>
       </c>
-      <c r="E16" t="str">
+      <c r="E16">
         <f>IF(test1!$C16=$D$4,test1!$E16,"")</f>
         <v/>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" t="str">
+      <c r="A17">
         <f>IF(test1!$C17=$A$4,test1!$D17,"")</f>
         <v/>
       </c>
-      <c r="B17" t="str">
+      <c r="B17">
         <f>IF(test1!$C17=$A$4,test1!$E17,"")</f>
         <v/>
       </c>
-      <c r="D17" t="str">
+      <c r="D17">
         <f>IF(test1!$C17=$D$4,test1!$D17,"")</f>
         <v/>
       </c>
-      <c r="E17" t="str">
+      <c r="E17">
         <f>IF(test1!$C17=$D$4,test1!$E17,"")</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" t="str">
+      <c r="A18">
         <f>IF(test1!$C18=$A$4,test1!$D18,"")</f>
         <v/>
       </c>
-      <c r="B18" t="str">
+      <c r="B18">
         <f>IF(test1!$C18=$A$4,test1!$E18,"")</f>
         <v/>
       </c>
-      <c r="D18" t="str">
+      <c r="D18">
         <f>IF(test1!$C18=$D$4,test1!$D18,"")</f>
         <v/>
       </c>
-      <c r="E18" t="str">
+      <c r="E18">
         <f>IF(test1!$C18=$D$4,test1!$E18,"")</f>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" t="str">
+      <c r="A19">
         <f>IF(test1!$C19=$A$4,test1!$D19,"")</f>
         <v/>
       </c>
-      <c r="B19" t="str">
+      <c r="B19">
         <f>IF(test1!$C19=$A$4,test1!$E19,"")</f>
         <v/>
       </c>
-      <c r="D19" t="str">
+      <c r="D19">
         <f>IF(test1!$C19=$D$4,test1!$D19,"")</f>
         <v/>
       </c>
-      <c r="E19" t="str">
+      <c r="E19">
         <f>IF(test1!$C19=$D$4,test1!$E19,"")</f>
         <v/>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" t="str">
+      <c r="A20">
         <f>IF(test1!$C20=$A$4,test1!$D20,"")</f>
         <v/>
       </c>
-      <c r="B20" t="str">
+      <c r="B20">
         <f>IF(test1!$C20=$A$4,test1!$E20,"")</f>
         <v/>
       </c>
-      <c r="D20" t="str">
+      <c r="D20">
         <f>IF(test1!$C20=$D$4,test1!$D20,"")</f>
         <v/>
       </c>
-      <c r="E20" t="str">
+      <c r="E20">
         <f>IF(test1!$C20=$D$4,test1!$E20,"")</f>
         <v/>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" t="str">
+      <c r="A21">
         <f>IF(test1!$C21=$A$4,test1!$D21,"")</f>
         <v/>
       </c>
-      <c r="B21" t="str">
+      <c r="B21">
         <f>IF(test1!$C21=$A$4,test1!$E21,"")</f>
         <v/>
       </c>
-      <c r="D21" t="str">
+      <c r="D21">
         <f>IF(test1!$C21=$D$4,test1!$D21,"")</f>
         <v/>
       </c>
-      <c r="E21" t="str">
+      <c r="E21">
         <f>IF(test1!$C21=$D$4,test1!$E21,"")</f>
         <v/>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" t="str">
+      <c r="A22">
         <f>IF(test1!$C22=$A$4,test1!$D22,"")</f>
         <v/>
       </c>
-      <c r="B22" t="str">
+      <c r="B22">
         <f>IF(test1!$C22=$A$4,test1!$E22,"")</f>
         <v/>
       </c>
-      <c r="D22" t="str">
+      <c r="D22">
         <f>IF(test1!$C22=$D$4,test1!$D22,"")</f>
         <v/>
       </c>
-      <c r="E22" t="str">
+      <c r="E22">
         <f>IF(test1!$C22=$D$4,test1!$E22,"")</f>
         <v/>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" t="str">
+      <c r="A23">
         <f>IF(test1!$C23=$A$4,test1!$D23,"")</f>
         <v/>
       </c>
-      <c r="B23" t="str">
+      <c r="B23">
         <f>IF(test1!$C23=$A$4,test1!$E23,"")</f>
         <v/>
       </c>
-      <c r="D23" t="str">
+      <c r="D23">
         <f>IF(test1!$C23=$D$4,test1!$D23,"")</f>
         <v/>
       </c>
-      <c r="E23" t="str">
+      <c r="E23">
         <f>IF(test1!$C23=$D$4,test1!$E23,"")</f>
         <v/>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" t="str">
+      <c r="A24">
         <f>IF(test1!$C24=$A$4,test1!$D24,"")</f>
         <v/>
       </c>
-      <c r="B24" t="str">
+      <c r="B24">
         <f>IF(test1!$C24=$A$4,test1!$E24,"")</f>
         <v/>
       </c>
-      <c r="D24" t="str">
+      <c r="D24">
         <f>IF(test1!$C24=$D$4,test1!$D24,"")</f>
         <v/>
       </c>
-      <c r="E24" t="str">
+      <c r="E24">
         <f>IF(test1!$C24=$D$4,test1!$E24,"")</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup copies="0" horizontalDpi="0" orientation="portrait" paperSize="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>